<commit_message>
add Genetic algorithm to optimize weights
</commit_message>
<xml_diff>
--- a/Result/result4.xlsx
+++ b/Result/result4.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IIM\工研院計畫\ITRI_2018\Result\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IIM\工研院計畫\ITRI_2018\OTA\Result\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1050,7 +1050,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="B2" sqref="B2:D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1091,7 +1091,7 @@
         <v>28</v>
       </c>
       <c r="B2" s="1">
-        <v>844.76944303475102</v>
+        <v>1</v>
       </c>
       <c r="C2" s="1">
         <v>869.56859327794496</v>

</xml_diff>